<commit_message>
Adição da coluna de subcategorias
</commit_message>
<xml_diff>
--- a/tweets_Nintendo_201809042125.xlsx
+++ b/tweets_Nintendo_201809042125.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Enrico Aloisi Nardi\Desktop\Insper\SEGUNDO semestre\Ciência dos Dados\PROJETO 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jadson\Desktop\Insper\Ciência dos dados\Projeto2CDD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C6D102DC-6D4C-49F1-AAC7-CC10E1E235B8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25AC170A-92CD-409D-AC8F-E9314F1D8203}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="21600" windowHeight="9510" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="21600" windowHeight="9510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1387" uniqueCount="453">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1389" uniqueCount="455">
   <si>
     <t>Treinamento</t>
   </si>
@@ -1515,6 +1515,12 @@
   </si>
   <si>
     <t>Classificação (B M)</t>
+  </si>
+  <si>
+    <t>Classificação Final</t>
+  </si>
+  <si>
+    <t>Classificação Sub (MR, R, N, I, MI)</t>
   </si>
 </sst>
 </file>
@@ -1931,19 +1937,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:D301"/>
   <sheetViews>
-    <sheetView topLeftCell="A153" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A203" sqref="A203"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="192.28515625" customWidth="1"/>
+    <col min="1" max="1" width="52.28515625" customWidth="1"/>
     <col min="2" max="3" width="17.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1953,8 +1960,11 @@
       <c r="C1" s="2" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1965,7 +1975,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1976,7 +1986,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1987,7 +1997,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1995,7 +2005,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -2003,7 +2013,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -2014,7 +2024,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -2025,7 +2035,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -2036,7 +2046,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -2044,7 +2054,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -2052,7 +2062,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -2063,7 +2073,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -2074,7 +2084,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -2085,7 +2095,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -2096,7 +2106,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -2506,7 +2516,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>50</v>
       </c>
@@ -5054,20 +5064,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C201"/>
+  <dimension ref="A1:D201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A140" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C157" sqref="C157"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="182.7109375" customWidth="1"/>
+    <col min="1" max="1" width="90.42578125" customWidth="1"/>
     <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>272</v>
       </c>
@@ -5077,8 +5088,11 @@
       <c r="C1" s="2" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>273</v>
       </c>
@@ -5086,7 +5100,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>274</v>
       </c>
@@ -5094,7 +5108,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>275</v>
       </c>
@@ -5105,7 +5119,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>276</v>
       </c>
@@ -5116,7 +5130,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>277</v>
       </c>
@@ -5127,7 +5141,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>278</v>
       </c>
@@ -5138,7 +5152,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>279</v>
       </c>
@@ -5149,7 +5163,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>280</v>
       </c>
@@ -5160,7 +5174,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>281</v>
       </c>
@@ -5171,7 +5185,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>282</v>
       </c>
@@ -5182,7 +5196,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>283</v>
       </c>
@@ -5193,7 +5207,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>284</v>
       </c>
@@ -5204,7 +5218,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>285</v>
       </c>
@@ -5215,7 +5229,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>286</v>
       </c>
@@ -5226,7 +5240,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>287</v>
       </c>

</xml_diff>

<commit_message>
recebendo a base de testes
</commit_message>
<xml_diff>
--- a/tweets_Nintendo_201809042125.xlsx
+++ b/tweets_Nintendo_201809042125.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jadson\Desktop\Insper\Ciência dos dados\Projeto2CDD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B266AAD-574A-4A92-B50D-CE8D23C158DA}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D64235FC-9DC8-4A71-A460-4C5EB8210303}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="600" windowWidth="21600" windowHeight="9510" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5972,8 +5972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A194" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D163" sqref="D163"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J146" sqref="J146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>